<commit_message>
Added 4 players to the file
</commit_message>
<xml_diff>
--- a/registered players.xlsx
+++ b/registered players.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="17">
   <si>
     <t>Name</t>
   </si>
@@ -54,6 +54,27 @@
   </si>
   <si>
     <t>motsobreakstyle@gmail.com</t>
+  </si>
+  <si>
+    <t>Eloundou Yvan</t>
+  </si>
+  <si>
+    <t>L1C</t>
+  </si>
+  <si>
+    <t>Kemta Tchoffo</t>
+  </si>
+  <si>
+    <t>Ndoum Junior</t>
+  </si>
+  <si>
+    <t>Bobo Benda Ulrich Gregore</t>
+  </si>
+  <si>
+    <t>L1A</t>
+  </si>
+  <si>
+    <t>Assoumou Assoumou Alahn</t>
   </si>
 </sst>
 </file>
@@ -382,15 +403,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="26.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.42578125" bestFit="1" customWidth="1"/>
@@ -441,6 +462,61 @@
         <v>9</v>
       </c>
     </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4">
+        <v>698207148</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5">
+        <v>656773516</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6">
+        <v>653303192</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7">
+        <v>699003156</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8">
+        <v>696715079</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1"/>

</xml_diff>

<commit_message>
A better looking more customizable bracket
</commit_message>
<xml_diff>
--- a/registered players.xlsx
+++ b/registered players.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="24">
   <si>
     <t>Name</t>
   </si>
@@ -75,6 +75,27 @@
   </si>
   <si>
     <t>Assoumou Assoumou Alahn</t>
+  </si>
+  <si>
+    <t>Hanj Manfred Elakie Ngalle</t>
+  </si>
+  <si>
+    <t>B1B</t>
+  </si>
+  <si>
+    <t>Kouayep Wanko Ruchi</t>
+  </si>
+  <si>
+    <t>Yvan Longo Gaetan Simon</t>
+  </si>
+  <si>
+    <t>B1A</t>
+  </si>
+  <si>
+    <t>Nzoga Gilbert Boris</t>
+  </si>
+  <si>
+    <t>L1E</t>
   </si>
 </sst>
 </file>
@@ -403,10 +424,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -517,6 +538,50 @@
         <v>696715079</v>
       </c>
     </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9">
+        <v>650469243</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10">
+        <v>695353905</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11">
+        <v>691674935</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12">
+        <v>657046719</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1"/>

</xml_diff>

<commit_message>
Put the server URL in every AJAX request
</commit_message>
<xml_diff>
--- a/registered players.xlsx
+++ b/registered players.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="25">
   <si>
     <t>Name</t>
   </si>
@@ -96,6 +96,9 @@
   </si>
   <si>
     <t>L1E</t>
+  </si>
+  <si>
+    <t>Tsembom Percy</t>
   </si>
 </sst>
 </file>
@@ -424,10 +427,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -582,6 +585,17 @@
         <v>657046719</v>
       </c>
     </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13">
+        <v>692201677</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1"/>

</xml_diff>